<commit_message>
loads almost all datasets. Still working on phys&health features
</commit_message>
<xml_diff>
--- a/MSF Dataset_450/MSF_Physical&health_Fetaures_450.xlsx
+++ b/MSF Dataset_450/MSF_Physical&health_Fetaures_450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/himanideshpande/Desktop/IEEE_data_submission/MSF Dataset_400/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\PROJECTS\MotherSignificantFeatureProject\MSF Dataset_450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C9D58F-5576-534C-8EE2-6580D1920ACC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DCE03C-45B5-48C4-8BD2-619E5C6A7E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="500" windowWidth="27240" windowHeight="15340" xr2:uid="{7336C592-27FA-9B4D-AC7E-FCD488218963}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7336C592-27FA-9B4D-AC7E-FCD488218963}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -903,33 +912,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AF3304-3CB7-AC49-A322-55F998F09B37}">
   <dimension ref="A1:X456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A449" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B463" sqref="B463"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A448" sqref="A448"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="6.33203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="6.375" style="8" customWidth="1"/>
     <col min="3" max="3" width="7" style="8" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="5.875" style="8" customWidth="1"/>
     <col min="5" max="5" width="10" style="10" customWidth="1"/>
-    <col min="6" max="6" width="5.1640625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="10"/>
-    <col min="8" max="8" width="6.1640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="10"/>
-    <col min="10" max="10" width="7.6640625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="7.83203125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="3.33203125" style="12" customWidth="1"/>
-    <col min="14" max="14" width="5.83203125" style="13" customWidth="1"/>
-    <col min="15" max="21" width="5.83203125" style="8" customWidth="1"/>
-    <col min="22" max="22" width="5.83203125" style="32" customWidth="1"/>
-    <col min="23" max="24" width="5.83203125" style="14" customWidth="1"/>
-    <col min="25" max="16384" width="10.83203125" style="8"/>
+    <col min="6" max="6" width="5.125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="10"/>
+    <col min="8" max="8" width="6.125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="10"/>
+    <col min="10" max="10" width="7.625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="7.875" style="10" customWidth="1"/>
+    <col min="12" max="12" width="3.125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="17.25" style="12" customWidth="1"/>
+    <col min="14" max="14" width="5.875" style="13" customWidth="1"/>
+    <col min="15" max="21" width="5.875" style="8" customWidth="1"/>
+    <col min="22" max="22" width="5.875" style="32" customWidth="1"/>
+    <col min="23" max="24" width="5.875" style="14" customWidth="1"/>
+    <col min="25" max="16384" width="10.875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="37" t="s">
         <v>0</v>
@@ -981,7 +990,7 @@
       <c r="W1" s="5"/>
       <c r="X1" s="7"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="37">
         <v>1</v>
@@ -1053,7 +1062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" s="40">
         <v>1</v>
       </c>
@@ -1146,7 +1155,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="41" t="s">
@@ -1181,7 +1190,7 @@
       <c r="W4" s="1"/>
       <c r="X4" s="10"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L5" s="44">
         <v>12</v>
       </c>
@@ -1216,7 +1225,7 @@
       <c r="W5" s="1"/>
       <c r="X5" s="10"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -1335,7 +1344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>A7+1</f>
         <v>2</v>
@@ -1411,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" ref="A9:A72" si="3">A8+1</f>
         <v>3</v>
@@ -1487,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -1563,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -1639,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -1715,7 +1724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1791,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -1867,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1943,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -2019,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -2095,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -2171,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -2247,7 +2256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -2323,7 +2332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -2399,7 +2408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -2475,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -2551,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -2627,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -2703,7 +2712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -2779,7 +2788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -2855,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -2931,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -3007,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -3083,7 +3092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -3159,7 +3168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -3235,7 +3244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -3311,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -3387,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -3463,7 +3472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -3539,7 +3548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -3615,7 +3624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -3691,7 +3700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -3767,7 +3776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -3843,7 +3852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -3919,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -3995,7 +4004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f t="shared" si="3"/>
         <v>37</v>
@@ -4071,7 +4080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <f t="shared" si="3"/>
         <v>38</v>
@@ -4147,7 +4156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f t="shared" si="3"/>
         <v>39</v>
@@ -4223,7 +4232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <f t="shared" si="3"/>
         <v>40</v>
@@ -4299,7 +4308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <f t="shared" si="3"/>
         <v>41</v>
@@ -4375,7 +4384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <f t="shared" si="3"/>
         <v>42</v>
@@ -4451,7 +4460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f t="shared" si="3"/>
         <v>43</v>
@@ -4527,7 +4536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <f t="shared" si="3"/>
         <v>44</v>
@@ -4603,7 +4612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -4679,7 +4688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <f t="shared" si="3"/>
         <v>46</v>
@@ -4755,7 +4764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -4831,7 +4840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -4907,7 +4916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -4983,7 +4992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -5059,7 +5068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <f t="shared" si="3"/>
         <v>51</v>
@@ -5135,7 +5144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <f t="shared" si="3"/>
         <v>52</v>
@@ -5211,7 +5220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <f t="shared" si="3"/>
         <v>53</v>
@@ -5287,7 +5296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <f t="shared" si="3"/>
         <v>54</v>
@@ -5363,7 +5372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <f t="shared" si="3"/>
         <v>55</v>
@@ -5439,7 +5448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <f t="shared" si="3"/>
         <v>56</v>
@@ -5515,7 +5524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <f t="shared" si="3"/>
         <v>57</v>
@@ -5591,7 +5600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <f t="shared" si="3"/>
         <v>58</v>
@@ -5667,7 +5676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <f t="shared" si="3"/>
         <v>59</v>
@@ -5743,7 +5752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <f t="shared" si="3"/>
         <v>60</v>
@@ -5819,7 +5828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <f t="shared" si="3"/>
         <v>61</v>
@@ -5895,7 +5904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <f t="shared" si="3"/>
         <v>62</v>
@@ -5971,7 +5980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <f t="shared" si="3"/>
         <v>63</v>
@@ -6047,7 +6056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <f t="shared" si="3"/>
         <v>64</v>
@@ -6123,7 +6132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <f t="shared" si="3"/>
         <v>65</v>
@@ -6199,7 +6208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <f t="shared" si="3"/>
         <v>66</v>
@@ -6275,7 +6284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <f t="shared" ref="A73:A136" si="5">A72+1</f>
         <v>67</v>
@@ -6351,7 +6360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <f t="shared" si="5"/>
         <v>68</v>
@@ -6427,7 +6436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <f t="shared" si="5"/>
         <v>69</v>
@@ -6503,7 +6512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <f t="shared" si="5"/>
         <v>70</v>
@@ -6579,7 +6588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <f t="shared" si="5"/>
         <v>71</v>
@@ -6655,7 +6664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <f t="shared" si="5"/>
         <v>72</v>
@@ -6731,7 +6740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <f t="shared" si="5"/>
         <v>73</v>
@@ -6807,7 +6816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <f t="shared" si="5"/>
         <v>74</v>
@@ -6883,7 +6892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <f t="shared" si="5"/>
         <v>75</v>
@@ -6959,7 +6968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <f t="shared" si="5"/>
         <v>76</v>
@@ -7035,7 +7044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <f t="shared" si="5"/>
         <v>77</v>
@@ -7111,7 +7120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <f t="shared" si="5"/>
         <v>78</v>
@@ -7187,7 +7196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <f t="shared" si="5"/>
         <v>79</v>
@@ -7263,7 +7272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <f t="shared" si="5"/>
         <v>80</v>
@@ -7339,7 +7348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <f t="shared" si="5"/>
         <v>81</v>
@@ -7415,7 +7424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <f t="shared" si="5"/>
         <v>82</v>
@@ -7491,7 +7500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <f t="shared" si="5"/>
         <v>83</v>
@@ -7567,7 +7576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <f t="shared" si="5"/>
         <v>84</v>
@@ -7643,7 +7652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <f t="shared" si="5"/>
         <v>85</v>
@@ -7719,7 +7728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <f t="shared" si="5"/>
         <v>86</v>
@@ -7795,7 +7804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <f t="shared" si="5"/>
         <v>87</v>
@@ -7871,7 +7880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <f t="shared" si="5"/>
         <v>88</v>
@@ -7947,7 +7956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <f t="shared" si="5"/>
         <v>89</v>
@@ -8023,7 +8032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <f t="shared" si="5"/>
         <v>90</v>
@@ -8099,7 +8108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <f t="shared" si="5"/>
         <v>91</v>
@@ -8175,7 +8184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <f t="shared" si="5"/>
         <v>92</v>
@@ -8251,7 +8260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <f t="shared" si="5"/>
         <v>93</v>
@@ -8327,7 +8336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <f t="shared" si="5"/>
         <v>94</v>
@@ -8403,7 +8412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <f t="shared" si="5"/>
         <v>95</v>
@@ -8479,7 +8488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <f t="shared" si="5"/>
         <v>96</v>
@@ -8555,7 +8564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <f t="shared" si="5"/>
         <v>97</v>
@@ -8631,7 +8640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <f t="shared" si="5"/>
         <v>98</v>
@@ -8707,7 +8716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <f t="shared" si="5"/>
         <v>99</v>
@@ -8783,7 +8792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <f t="shared" si="5"/>
         <v>100</v>
@@ -8859,7 +8868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <f t="shared" si="5"/>
         <v>101</v>
@@ -8935,7 +8944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <f t="shared" si="5"/>
         <v>102</v>
@@ -9011,7 +9020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <f t="shared" si="5"/>
         <v>103</v>
@@ -9087,7 +9096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <f t="shared" si="5"/>
         <v>104</v>
@@ -9163,7 +9172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <f t="shared" si="5"/>
         <v>105</v>
@@ -9239,7 +9248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <f t="shared" si="5"/>
         <v>106</v>
@@ -9315,7 +9324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <f t="shared" si="5"/>
         <v>107</v>
@@ -9391,7 +9400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <f t="shared" si="5"/>
         <v>108</v>
@@ -9467,7 +9476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <f t="shared" si="5"/>
         <v>109</v>
@@ -9543,7 +9552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <f t="shared" si="5"/>
         <v>110</v>
@@ -9619,7 +9628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <f t="shared" si="5"/>
         <v>111</v>
@@ -9695,7 +9704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <f t="shared" si="5"/>
         <v>112</v>
@@ -9771,7 +9780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <f t="shared" si="5"/>
         <v>113</v>
@@ -9847,7 +9856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <f t="shared" si="5"/>
         <v>114</v>
@@ -9923,7 +9932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <f t="shared" si="5"/>
         <v>115</v>
@@ -9999,7 +10008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <f t="shared" si="5"/>
         <v>116</v>
@@ -10075,7 +10084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <f t="shared" si="5"/>
         <v>117</v>
@@ -10151,7 +10160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <f t="shared" si="5"/>
         <v>118</v>
@@ -10227,7 +10236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <f t="shared" si="5"/>
         <v>119</v>
@@ -10303,7 +10312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <f t="shared" si="5"/>
         <v>120</v>
@@ -10379,7 +10388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <f t="shared" si="5"/>
         <v>121</v>
@@ -10455,7 +10464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <f t="shared" si="5"/>
         <v>122</v>
@@ -10531,7 +10540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <f t="shared" si="5"/>
         <v>123</v>
@@ -10607,7 +10616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <f t="shared" si="5"/>
         <v>124</v>
@@ -10683,7 +10692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <f t="shared" si="5"/>
         <v>125</v>
@@ -10759,7 +10768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <f t="shared" si="5"/>
         <v>126</v>
@@ -10835,7 +10844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <f t="shared" si="5"/>
         <v>127</v>
@@ -10911,7 +10920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <f t="shared" si="5"/>
         <v>128</v>
@@ -10987,7 +10996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <f t="shared" si="5"/>
         <v>129</v>
@@ -11063,7 +11072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <f t="shared" si="5"/>
         <v>130</v>
@@ -11139,7 +11148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <f t="shared" ref="A137:A200" si="7">A136+1</f>
         <v>131</v>
@@ -11215,7 +11224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <f t="shared" si="7"/>
         <v>132</v>
@@ -11291,7 +11300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <f t="shared" si="7"/>
         <v>133</v>
@@ -11367,7 +11376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <f t="shared" si="7"/>
         <v>134</v>
@@ -11443,7 +11452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <f t="shared" si="7"/>
         <v>135</v>
@@ -11519,7 +11528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <f t="shared" si="7"/>
         <v>136</v>
@@ -11595,7 +11604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <f t="shared" si="7"/>
         <v>137</v>
@@ -11671,7 +11680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <f t="shared" si="7"/>
         <v>138</v>
@@ -11747,7 +11756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <f t="shared" si="7"/>
         <v>139</v>
@@ -11823,7 +11832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <f t="shared" si="7"/>
         <v>140</v>
@@ -11899,7 +11908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <f t="shared" si="7"/>
         <v>141</v>
@@ -11975,7 +11984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <f t="shared" si="7"/>
         <v>142</v>
@@ -12051,7 +12060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <f t="shared" si="7"/>
         <v>143</v>
@@ -12127,7 +12136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <f t="shared" si="7"/>
         <v>144</v>
@@ -12203,7 +12212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <f t="shared" si="7"/>
         <v>145</v>
@@ -12279,7 +12288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <f t="shared" si="7"/>
         <v>146</v>
@@ -12355,7 +12364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <f t="shared" si="7"/>
         <v>147</v>
@@ -12431,7 +12440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <f t="shared" si="7"/>
         <v>148</v>
@@ -12507,7 +12516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <f t="shared" si="7"/>
         <v>149</v>
@@ -12583,7 +12592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <f t="shared" si="7"/>
         <v>150</v>
@@ -12659,7 +12668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <f t="shared" si="7"/>
         <v>151</v>
@@ -12735,7 +12744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <f t="shared" si="7"/>
         <v>152</v>
@@ -12811,7 +12820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <f t="shared" si="7"/>
         <v>153</v>
@@ -12887,7 +12896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <f t="shared" si="7"/>
         <v>154</v>
@@ -12963,7 +12972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <f t="shared" si="7"/>
         <v>155</v>
@@ -13039,7 +13048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <f t="shared" si="7"/>
         <v>156</v>
@@ -13115,7 +13124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <f t="shared" si="7"/>
         <v>157</v>
@@ -13191,7 +13200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <f t="shared" si="7"/>
         <v>158</v>
@@ -13267,7 +13276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <f t="shared" si="7"/>
         <v>159</v>
@@ -13343,7 +13352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <f t="shared" si="7"/>
         <v>160</v>
@@ -13419,7 +13428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <f t="shared" si="7"/>
         <v>161</v>
@@ -13495,7 +13504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <f t="shared" si="7"/>
         <v>162</v>
@@ -13571,7 +13580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <f t="shared" si="7"/>
         <v>163</v>
@@ -13647,7 +13656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <f t="shared" si="7"/>
         <v>164</v>
@@ -13723,7 +13732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <f t="shared" si="7"/>
         <v>165</v>
@@ -13799,7 +13808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <f t="shared" si="7"/>
         <v>166</v>
@@ -13875,7 +13884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <f t="shared" si="7"/>
         <v>167</v>
@@ -13951,7 +13960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <f t="shared" si="7"/>
         <v>168</v>
@@ -14027,7 +14036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <f t="shared" si="7"/>
         <v>169</v>
@@ -14103,7 +14112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <f t="shared" si="7"/>
         <v>170</v>
@@ -14179,7 +14188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <f t="shared" si="7"/>
         <v>171</v>
@@ -14255,7 +14264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <f t="shared" si="7"/>
         <v>172</v>
@@ -14331,7 +14340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <f t="shared" si="7"/>
         <v>173</v>
@@ -14407,7 +14416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <f t="shared" si="7"/>
         <v>174</v>
@@ -14483,7 +14492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <f t="shared" si="7"/>
         <v>175</v>
@@ -14559,7 +14568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <f t="shared" si="7"/>
         <v>176</v>
@@ -14635,7 +14644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <f t="shared" si="7"/>
         <v>177</v>
@@ -14711,7 +14720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <f t="shared" si="7"/>
         <v>178</v>
@@ -14787,7 +14796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <f t="shared" si="7"/>
         <v>179</v>
@@ -14863,7 +14872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <f t="shared" si="7"/>
         <v>180</v>
@@ -14939,7 +14948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <f t="shared" si="7"/>
         <v>181</v>
@@ -15015,7 +15024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <f t="shared" si="7"/>
         <v>182</v>
@@ -15091,7 +15100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <f t="shared" si="7"/>
         <v>183</v>
@@ -15167,7 +15176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <f t="shared" si="7"/>
         <v>184</v>
@@ -15243,7 +15252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <f t="shared" si="7"/>
         <v>185</v>
@@ -15319,7 +15328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <f t="shared" si="7"/>
         <v>186</v>
@@ -15395,7 +15404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <f t="shared" si="7"/>
         <v>187</v>
@@ -15471,7 +15480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <f t="shared" si="7"/>
         <v>188</v>
@@ -15547,7 +15556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <f t="shared" si="7"/>
         <v>189</v>
@@ -15623,7 +15632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <f t="shared" si="7"/>
         <v>190</v>
@@ -15699,7 +15708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <f t="shared" si="7"/>
         <v>191</v>
@@ -15775,7 +15784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <f t="shared" si="7"/>
         <v>192</v>
@@ -15851,7 +15860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <f t="shared" si="7"/>
         <v>193</v>
@@ -15927,7 +15936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <f t="shared" si="7"/>
         <v>194</v>
@@ -16003,7 +16012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <f t="shared" ref="A201:A264" si="8">A200+1</f>
         <v>195</v>
@@ -16079,7 +16088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <f t="shared" si="8"/>
         <v>196</v>
@@ -16155,7 +16164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <f t="shared" si="8"/>
         <v>197</v>
@@ -16231,7 +16240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <f t="shared" si="8"/>
         <v>198</v>
@@ -16307,7 +16316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <f t="shared" si="8"/>
         <v>199</v>
@@ -16383,7 +16392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <f t="shared" si="8"/>
         <v>200</v>
@@ -16459,7 +16468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <f t="shared" si="8"/>
         <v>201</v>
@@ -16529,7 +16538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <f t="shared" si="8"/>
         <v>202</v>
@@ -16599,7 +16608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <f t="shared" si="8"/>
         <v>203</v>
@@ -16669,7 +16678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <f t="shared" si="8"/>
         <v>204</v>
@@ -16739,7 +16748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <f t="shared" si="8"/>
         <v>205</v>
@@ -16809,7 +16818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <f t="shared" si="8"/>
         <v>206</v>
@@ -16879,7 +16888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <f t="shared" si="8"/>
         <v>207</v>
@@ -16949,7 +16958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <f t="shared" si="8"/>
         <v>208</v>
@@ -17019,7 +17028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <f t="shared" si="8"/>
         <v>209</v>
@@ -17089,7 +17098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <f t="shared" si="8"/>
         <v>210</v>
@@ -17159,7 +17168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <f t="shared" si="8"/>
         <v>211</v>
@@ -17229,7 +17238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <f t="shared" si="8"/>
         <v>212</v>
@@ -17299,7 +17308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <f t="shared" si="8"/>
         <v>213</v>
@@ -17369,7 +17378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <f t="shared" si="8"/>
         <v>214</v>
@@ -17439,7 +17448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <f t="shared" si="8"/>
         <v>215</v>
@@ -17509,7 +17518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <f t="shared" si="8"/>
         <v>216</v>
@@ -17579,7 +17588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <f t="shared" si="8"/>
         <v>217</v>
@@ -17649,7 +17658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <f t="shared" si="8"/>
         <v>218</v>
@@ -17719,7 +17728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <f t="shared" si="8"/>
         <v>219</v>
@@ -17789,7 +17798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <f t="shared" si="8"/>
         <v>220</v>
@@ -17859,7 +17868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <f t="shared" si="8"/>
         <v>221</v>
@@ -17929,7 +17938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <f t="shared" si="8"/>
         <v>222</v>
@@ -17999,7 +18008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <f t="shared" si="8"/>
         <v>223</v>
@@ -18069,7 +18078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <f t="shared" si="8"/>
         <v>224</v>
@@ -18139,7 +18148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <f t="shared" si="8"/>
         <v>225</v>
@@ -18209,7 +18218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <f t="shared" si="8"/>
         <v>226</v>
@@ -18279,7 +18288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <f t="shared" si="8"/>
         <v>227</v>
@@ -18349,7 +18358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <f t="shared" si="8"/>
         <v>228</v>
@@ -18419,7 +18428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <f t="shared" si="8"/>
         <v>229</v>
@@ -18489,7 +18498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <f t="shared" si="8"/>
         <v>230</v>
@@ -18559,7 +18568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <f t="shared" si="8"/>
         <v>231</v>
@@ -18629,7 +18638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <f t="shared" si="8"/>
         <v>232</v>
@@ -18699,7 +18708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <f t="shared" si="8"/>
         <v>233</v>
@@ -18769,7 +18778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <f t="shared" si="8"/>
         <v>234</v>
@@ -18839,7 +18848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <f t="shared" si="8"/>
         <v>235</v>
@@ -18909,7 +18918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <f t="shared" si="8"/>
         <v>236</v>
@@ -18979,7 +18988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <f t="shared" si="8"/>
         <v>237</v>
@@ -19049,7 +19058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <f t="shared" si="8"/>
         <v>238</v>
@@ -19119,7 +19128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <f t="shared" si="8"/>
         <v>239</v>
@@ -19189,7 +19198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <f t="shared" si="8"/>
         <v>240</v>
@@ -19259,7 +19268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <f t="shared" si="8"/>
         <v>241</v>
@@ -19329,7 +19338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <f t="shared" si="8"/>
         <v>242</v>
@@ -19399,7 +19408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <f t="shared" si="8"/>
         <v>243</v>
@@ -19469,7 +19478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <f t="shared" si="8"/>
         <v>244</v>
@@ -19539,7 +19548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <f t="shared" si="8"/>
         <v>245</v>
@@ -19609,7 +19618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <f t="shared" si="8"/>
         <v>246</v>
@@ -19679,7 +19688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <f t="shared" si="8"/>
         <v>247</v>
@@ -19749,7 +19758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <f t="shared" si="8"/>
         <v>248</v>
@@ -19819,7 +19828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <f t="shared" si="8"/>
         <v>249</v>
@@ -19889,7 +19898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <f t="shared" si="8"/>
         <v>250</v>
@@ -19959,7 +19968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <f t="shared" si="8"/>
         <v>251</v>
@@ -20029,7 +20038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
         <f t="shared" si="8"/>
         <v>252</v>
@@ -20099,7 +20108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <f t="shared" si="8"/>
         <v>253</v>
@@ -20169,7 +20178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <f t="shared" si="8"/>
         <v>254</v>
@@ -20239,7 +20248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <f t="shared" si="8"/>
         <v>255</v>
@@ -20309,7 +20318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <f t="shared" si="8"/>
         <v>256</v>
@@ -20379,7 +20388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <f t="shared" si="8"/>
         <v>257</v>
@@ -20449,7 +20458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <f t="shared" si="8"/>
         <v>258</v>
@@ -20519,7 +20528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <f t="shared" ref="A265:A328" si="10">A264+1</f>
         <v>259</v>
@@ -20589,7 +20598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <f t="shared" si="10"/>
         <v>260</v>
@@ -20659,7 +20668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <f t="shared" si="10"/>
         <v>261</v>
@@ -20729,7 +20738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <f t="shared" si="10"/>
         <v>262</v>
@@ -20799,7 +20808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
         <f t="shared" si="10"/>
         <v>263</v>
@@ -20869,7 +20878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
         <f t="shared" si="10"/>
         <v>264</v>
@@ -20939,7 +20948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
         <f t="shared" si="10"/>
         <v>265</v>
@@ -21009,7 +21018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A272" s="2">
         <f t="shared" si="10"/>
         <v>266</v>
@@ -21079,7 +21088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A273" s="2">
         <f t="shared" si="10"/>
         <v>267</v>
@@ -21149,7 +21158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A274" s="2">
         <f t="shared" si="10"/>
         <v>268</v>
@@ -21219,7 +21228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A275" s="2">
         <f t="shared" si="10"/>
         <v>269</v>
@@ -21289,7 +21298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A276" s="2">
         <f t="shared" si="10"/>
         <v>270</v>
@@ -21359,7 +21368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
         <f t="shared" si="10"/>
         <v>271</v>
@@ -21429,7 +21438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
         <f t="shared" si="10"/>
         <v>272</v>
@@ -21499,7 +21508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A279" s="2">
         <f t="shared" si="10"/>
         <v>273</v>
@@ -21569,7 +21578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A280" s="2">
         <f t="shared" si="10"/>
         <v>274</v>
@@ -21639,7 +21648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A281" s="2">
         <f t="shared" si="10"/>
         <v>275</v>
@@ -21709,7 +21718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A282" s="2">
         <f t="shared" si="10"/>
         <v>276</v>
@@ -21779,7 +21788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A283" s="2">
         <f t="shared" si="10"/>
         <v>277</v>
@@ -21849,7 +21858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A284" s="2">
         <f t="shared" si="10"/>
         <v>278</v>
@@ -21919,7 +21928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
         <f t="shared" si="10"/>
         <v>279</v>
@@ -21989,7 +21998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
         <f t="shared" si="10"/>
         <v>280</v>
@@ -22059,7 +22068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
         <f t="shared" si="10"/>
         <v>281</v>
@@ -22129,7 +22138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
         <f t="shared" si="10"/>
         <v>282</v>
@@ -22199,7 +22208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A289" s="2">
         <f t="shared" si="10"/>
         <v>283</v>
@@ -22269,7 +22278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A290" s="2">
         <f t="shared" si="10"/>
         <v>284</v>
@@ -22339,7 +22348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A291" s="2">
         <f t="shared" si="10"/>
         <v>285</v>
@@ -22409,7 +22418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A292" s="2">
         <f t="shared" si="10"/>
         <v>286</v>
@@ -22479,7 +22488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A293" s="2">
         <f t="shared" si="10"/>
         <v>287</v>
@@ -22549,7 +22558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A294" s="2">
         <f t="shared" si="10"/>
         <v>288</v>
@@ -22619,7 +22628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A295" s="2">
         <f t="shared" si="10"/>
         <v>289</v>
@@ -22689,7 +22698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A296" s="2">
         <f t="shared" si="10"/>
         <v>290</v>
@@ -22759,7 +22768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <f t="shared" si="10"/>
         <v>291</v>
@@ -22829,7 +22838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <f t="shared" si="10"/>
         <v>292</v>
@@ -22899,7 +22908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A299" s="2">
         <f t="shared" si="10"/>
         <v>293</v>
@@ -22969,7 +22978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A300" s="2">
         <f t="shared" si="10"/>
         <v>294</v>
@@ -23039,7 +23048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A301" s="2">
         <f t="shared" si="10"/>
         <v>295</v>
@@ -23109,7 +23118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A302" s="2">
         <f t="shared" si="10"/>
         <v>296</v>
@@ -23179,7 +23188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A303" s="2">
         <f t="shared" si="10"/>
         <v>297</v>
@@ -23249,7 +23258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A304" s="2">
         <f t="shared" si="10"/>
         <v>298</v>
@@ -23319,7 +23328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" s="2">
         <f t="shared" si="10"/>
         <v>299</v>
@@ -23389,7 +23398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
         <f t="shared" si="10"/>
         <v>300</v>
@@ -23459,7 +23468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
         <f t="shared" si="10"/>
         <v>301</v>
@@ -23529,7 +23538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
         <f t="shared" si="10"/>
         <v>302</v>
@@ -23599,7 +23608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
         <f t="shared" si="10"/>
         <v>303</v>
@@ -23669,7 +23678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
         <f t="shared" si="10"/>
         <v>304</v>
@@ -23739,7 +23748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A311" s="2">
         <f t="shared" si="10"/>
         <v>305</v>
@@ -23809,7 +23818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A312" s="2">
         <f t="shared" si="10"/>
         <v>306</v>
@@ -23879,7 +23888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
         <f t="shared" si="10"/>
         <v>307</v>
@@ -23949,7 +23958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
         <f t="shared" si="10"/>
         <v>308</v>
@@ -24019,7 +24028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A315" s="2">
         <f t="shared" si="10"/>
         <v>309</v>
@@ -24089,7 +24098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A316" s="2">
         <f t="shared" si="10"/>
         <v>310</v>
@@ -24159,7 +24168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A317" s="2">
         <f t="shared" si="10"/>
         <v>311</v>
@@ -24229,7 +24238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A318" s="2">
         <f t="shared" si="10"/>
         <v>312</v>
@@ -24299,7 +24308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A319" s="2">
         <f t="shared" si="10"/>
         <v>313</v>
@@ -24369,7 +24378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A320" s="2">
         <f t="shared" si="10"/>
         <v>314</v>
@@ -24439,7 +24448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A321" s="2">
         <f t="shared" si="10"/>
         <v>315</v>
@@ -24509,7 +24518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A322" s="2">
         <f t="shared" si="10"/>
         <v>316</v>
@@ -24579,7 +24588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A323" s="2">
         <f t="shared" si="10"/>
         <v>317</v>
@@ -24649,7 +24658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A324" s="2">
         <f t="shared" si="10"/>
         <v>318</v>
@@ -24719,7 +24728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A325" s="2">
         <f t="shared" si="10"/>
         <v>319</v>
@@ -24789,7 +24798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A326" s="2">
         <f t="shared" si="10"/>
         <v>320</v>
@@ -24859,7 +24868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A327" s="2">
         <f t="shared" si="10"/>
         <v>321</v>
@@ -24929,7 +24938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A328" s="2">
         <f t="shared" si="10"/>
         <v>322</v>
@@ -24999,7 +25008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A329" s="2">
         <f t="shared" ref="A329:A392" si="12">A328+1</f>
         <v>323</v>
@@ -25069,7 +25078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A330" s="2">
         <f t="shared" si="12"/>
         <v>324</v>
@@ -25139,7 +25148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A331" s="2">
         <f t="shared" si="12"/>
         <v>325</v>
@@ -25209,7 +25218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A332" s="2">
         <f t="shared" si="12"/>
         <v>326</v>
@@ -25279,7 +25288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A333" s="2">
         <f t="shared" si="12"/>
         <v>327</v>
@@ -25349,7 +25358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A334" s="2">
         <f t="shared" si="12"/>
         <v>328</v>
@@ -25419,7 +25428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A335" s="2">
         <f t="shared" si="12"/>
         <v>329</v>
@@ -25489,7 +25498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A336" s="2">
         <f t="shared" si="12"/>
         <v>330</v>
@@ -25559,7 +25568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A337" s="2">
         <f t="shared" si="12"/>
         <v>331</v>
@@ -25629,7 +25638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A338" s="2">
         <f t="shared" si="12"/>
         <v>332</v>
@@ -25699,7 +25708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A339" s="2">
         <f t="shared" si="12"/>
         <v>333</v>
@@ -25769,7 +25778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A340" s="2">
         <f t="shared" si="12"/>
         <v>334</v>
@@ -25839,7 +25848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A341" s="2">
         <f t="shared" si="12"/>
         <v>335</v>
@@ -25909,7 +25918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A342" s="2">
         <f t="shared" si="12"/>
         <v>336</v>
@@ -25979,7 +25988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A343" s="2">
         <f t="shared" si="12"/>
         <v>337</v>
@@ -26049,7 +26058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A344" s="2">
         <f t="shared" si="12"/>
         <v>338</v>
@@ -26119,7 +26128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A345" s="2">
         <f t="shared" si="12"/>
         <v>339</v>
@@ -26189,7 +26198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A346" s="2">
         <f t="shared" si="12"/>
         <v>340</v>
@@ -26259,7 +26268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A347" s="2">
         <f t="shared" si="12"/>
         <v>341</v>
@@ -26329,7 +26338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A348" s="2">
         <f t="shared" si="12"/>
         <v>342</v>
@@ -26399,7 +26408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A349" s="2">
         <f t="shared" si="12"/>
         <v>343</v>
@@ -26469,7 +26478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A350" s="2">
         <f t="shared" si="12"/>
         <v>344</v>
@@ -26539,7 +26548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A351" s="2">
         <f t="shared" si="12"/>
         <v>345</v>
@@ -26609,7 +26618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A352" s="2">
         <f t="shared" si="12"/>
         <v>346</v>
@@ -26679,7 +26688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A353" s="2">
         <f t="shared" si="12"/>
         <v>347</v>
@@ -26749,7 +26758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A354" s="2">
         <f t="shared" si="12"/>
         <v>348</v>
@@ -26819,7 +26828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A355" s="2">
         <f t="shared" si="12"/>
         <v>349</v>
@@ -26889,7 +26898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A356" s="2">
         <f t="shared" si="12"/>
         <v>350</v>
@@ -26959,7 +26968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A357" s="2">
         <f t="shared" si="12"/>
         <v>351</v>
@@ -27029,7 +27038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A358" s="2">
         <f t="shared" si="12"/>
         <v>352</v>
@@ -27099,7 +27108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A359" s="2">
         <f t="shared" si="12"/>
         <v>353</v>
@@ -27169,7 +27178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A360" s="2">
         <f t="shared" si="12"/>
         <v>354</v>
@@ -27239,7 +27248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A361" s="2">
         <f t="shared" si="12"/>
         <v>355</v>
@@ -27309,7 +27318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A362" s="2">
         <f t="shared" si="12"/>
         <v>356</v>
@@ -27379,7 +27388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A363" s="2">
         <f t="shared" si="12"/>
         <v>357</v>
@@ -27449,7 +27458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A364" s="2">
         <f t="shared" si="12"/>
         <v>358</v>
@@ -27519,7 +27528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A365" s="2">
         <f t="shared" si="12"/>
         <v>359</v>
@@ -27589,7 +27598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A366" s="2">
         <f t="shared" si="12"/>
         <v>360</v>
@@ -27659,7 +27668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A367" s="2">
         <f t="shared" si="12"/>
         <v>361</v>
@@ -27729,7 +27738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A368" s="2">
         <f t="shared" si="12"/>
         <v>362</v>
@@ -27799,7 +27808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A369" s="2">
         <f t="shared" si="12"/>
         <v>363</v>
@@ -27869,7 +27878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A370" s="2">
         <f t="shared" si="12"/>
         <v>364</v>
@@ -27939,7 +27948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A371" s="2">
         <f t="shared" si="12"/>
         <v>365</v>
@@ -28009,7 +28018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A372" s="2">
         <f t="shared" si="12"/>
         <v>366</v>
@@ -28079,7 +28088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="373" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A373" s="2">
         <f t="shared" si="12"/>
         <v>367</v>
@@ -28149,7 +28158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A374" s="2">
         <f t="shared" si="12"/>
         <v>368</v>
@@ -28219,7 +28228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A375" s="2">
         <f t="shared" si="12"/>
         <v>369</v>
@@ -28289,7 +28298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A376" s="2">
         <f t="shared" si="12"/>
         <v>370</v>
@@ -28359,7 +28368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A377" s="2">
         <f t="shared" si="12"/>
         <v>371</v>
@@ -28429,7 +28438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A378" s="2">
         <f t="shared" si="12"/>
         <v>372</v>
@@ -28499,7 +28508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A379" s="2">
         <f t="shared" si="12"/>
         <v>373</v>
@@ -28569,7 +28578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A380" s="2">
         <f t="shared" si="12"/>
         <v>374</v>
@@ -28639,7 +28648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="381" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A381" s="2">
         <f t="shared" si="12"/>
         <v>375</v>
@@ -28709,7 +28718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A382" s="2">
         <f t="shared" si="12"/>
         <v>376</v>
@@ -28779,7 +28788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A383" s="2">
         <f t="shared" si="12"/>
         <v>377</v>
@@ -28849,7 +28858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A384" s="2">
         <f t="shared" si="12"/>
         <v>378</v>
@@ -28919,7 +28928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A385" s="2">
         <f t="shared" si="12"/>
         <v>379</v>
@@ -28989,7 +28998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A386" s="2">
         <f t="shared" si="12"/>
         <v>380</v>
@@ -29059,7 +29068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A387" s="2">
         <f t="shared" si="12"/>
         <v>381</v>
@@ -29129,7 +29138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A388" s="2">
         <f t="shared" si="12"/>
         <v>382</v>
@@ -29199,7 +29208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A389" s="2">
         <f t="shared" si="12"/>
         <v>383</v>
@@ -29269,7 +29278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A390" s="2">
         <f t="shared" si="12"/>
         <v>384</v>
@@ -29339,7 +29348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A391" s="2">
         <f t="shared" si="12"/>
         <v>385</v>
@@ -29409,7 +29418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A392" s="2">
         <f t="shared" si="12"/>
         <v>386</v>
@@ -29479,7 +29488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A393" s="2">
         <f t="shared" ref="A393:A456" si="14">A392+1</f>
         <v>387</v>
@@ -29549,7 +29558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A394" s="2">
         <f t="shared" si="14"/>
         <v>388</v>
@@ -29619,7 +29628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A395" s="2">
         <f t="shared" si="14"/>
         <v>389</v>
@@ -29689,7 +29698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A396" s="2">
         <f t="shared" si="14"/>
         <v>390</v>
@@ -29759,7 +29768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A397" s="2">
         <f t="shared" si="14"/>
         <v>391</v>
@@ -29829,7 +29838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="398" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A398" s="2">
         <f t="shared" si="14"/>
         <v>392</v>
@@ -29899,7 +29908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A399" s="2">
         <f t="shared" si="14"/>
         <v>393</v>
@@ -29969,7 +29978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A400" s="2">
         <f t="shared" si="14"/>
         <v>394</v>
@@ -30039,7 +30048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="401" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A401" s="2">
         <f t="shared" si="14"/>
         <v>395</v>
@@ -30109,7 +30118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="402" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A402" s="2">
         <f t="shared" si="14"/>
         <v>396</v>
@@ -30179,7 +30188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A403" s="2">
         <f t="shared" si="14"/>
         <v>397</v>
@@ -30249,7 +30258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="404" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A404" s="2">
         <f t="shared" si="14"/>
         <v>398</v>
@@ -30319,7 +30328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="405" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A405" s="2">
         <f t="shared" si="14"/>
         <v>399</v>
@@ -30389,7 +30398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="406" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A406" s="2">
         <f t="shared" si="14"/>
         <v>400</v>
@@ -30459,7 +30468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A407" s="2">
         <f t="shared" si="14"/>
         <v>401</v>
@@ -30529,7 +30538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A408" s="2">
         <f t="shared" si="14"/>
         <v>402</v>
@@ -30599,7 +30608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A409" s="2">
         <f t="shared" si="14"/>
         <v>403</v>
@@ -30669,7 +30678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A410" s="2">
         <f t="shared" si="14"/>
         <v>404</v>
@@ -30739,7 +30748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="411" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A411" s="2">
         <f t="shared" si="14"/>
         <v>405</v>
@@ -30809,7 +30818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A412" s="2">
         <f t="shared" si="14"/>
         <v>406</v>
@@ -30879,7 +30888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="413" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A413" s="2">
         <f t="shared" si="14"/>
         <v>407</v>
@@ -30949,7 +30958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A414" s="2">
         <f t="shared" si="14"/>
         <v>408</v>
@@ -31019,7 +31028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A415" s="2">
         <f t="shared" si="14"/>
         <v>409</v>
@@ -31089,7 +31098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A416" s="2">
         <f t="shared" si="14"/>
         <v>410</v>
@@ -31159,7 +31168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A417" s="2">
         <f t="shared" si="14"/>
         <v>411</v>
@@ -31229,7 +31238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="418" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A418" s="2">
         <f t="shared" si="14"/>
         <v>412</v>
@@ -31299,7 +31308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A419" s="2">
         <f t="shared" si="14"/>
         <v>413</v>
@@ -31369,7 +31378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="420" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A420" s="2">
         <f t="shared" si="14"/>
         <v>414</v>
@@ -31439,7 +31448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="421" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A421" s="2">
         <f t="shared" si="14"/>
         <v>415</v>
@@ -31509,7 +31518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A422" s="2">
         <f t="shared" si="14"/>
         <v>416</v>
@@ -31579,7 +31588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="423" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A423" s="2">
         <f t="shared" si="14"/>
         <v>417</v>
@@ -31649,7 +31658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="424" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A424" s="2">
         <f t="shared" si="14"/>
         <v>418</v>
@@ -31719,7 +31728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="425" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A425" s="2">
         <f t="shared" si="14"/>
         <v>419</v>
@@ -31789,7 +31798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A426" s="2">
         <f t="shared" si="14"/>
         <v>420</v>
@@ -31859,7 +31868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A427" s="2">
         <f t="shared" si="14"/>
         <v>421</v>
@@ -31929,7 +31938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="428" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A428" s="2">
         <f t="shared" si="14"/>
         <v>422</v>
@@ -31999,7 +32008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A429" s="2">
         <f t="shared" si="14"/>
         <v>423</v>
@@ -32069,7 +32078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="430" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A430" s="2">
         <f t="shared" si="14"/>
         <v>424</v>
@@ -32139,7 +32148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A431" s="2">
         <f t="shared" si="14"/>
         <v>425</v>
@@ -32209,7 +32218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A432" s="2">
         <f t="shared" si="14"/>
         <v>426</v>
@@ -32279,7 +32288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A433" s="2">
         <f t="shared" si="14"/>
         <v>427</v>
@@ -32349,7 +32358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A434" s="2">
         <f t="shared" si="14"/>
         <v>428</v>
@@ -32419,7 +32428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A435" s="2">
         <f t="shared" si="14"/>
         <v>429</v>
@@ -32489,7 +32498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A436" s="2">
         <f t="shared" si="14"/>
         <v>430</v>
@@ -32559,7 +32568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="437" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A437" s="2">
         <f t="shared" si="14"/>
         <v>431</v>
@@ -32629,7 +32638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A438" s="2">
         <f t="shared" si="14"/>
         <v>432</v>
@@ -32699,7 +32708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A439" s="2">
         <f t="shared" si="14"/>
         <v>433</v>
@@ -32769,7 +32778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="440" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A440" s="2">
         <f t="shared" si="14"/>
         <v>434</v>
@@ -32839,7 +32848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A441" s="2">
         <f t="shared" si="14"/>
         <v>435</v>
@@ -32909,7 +32918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="442" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A442" s="2">
         <f t="shared" si="14"/>
         <v>436</v>
@@ -32979,7 +32988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="443" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A443" s="2">
         <f t="shared" si="14"/>
         <v>437</v>
@@ -33049,7 +33058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="444" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A444" s="2">
         <f t="shared" si="14"/>
         <v>438</v>
@@ -33119,7 +33128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="445" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A445" s="2">
         <f t="shared" si="14"/>
         <v>439</v>
@@ -33189,7 +33198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="446" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A446" s="2">
         <f t="shared" si="14"/>
         <v>440</v>
@@ -33259,7 +33268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="447" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A447" s="2">
         <f t="shared" si="14"/>
         <v>441</v>
@@ -33329,7 +33338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="448" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A448" s="2">
         <f t="shared" si="14"/>
         <v>442</v>
@@ -33399,7 +33408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="449" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A449" s="2">
         <f t="shared" si="14"/>
         <v>443</v>
@@ -33469,7 +33478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="450" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A450" s="2">
         <f t="shared" si="14"/>
         <v>444</v>
@@ -33539,7 +33548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="451" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A451" s="2">
         <f t="shared" si="14"/>
         <v>445</v>
@@ -33609,7 +33618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="452" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A452" s="2">
         <f t="shared" si="14"/>
         <v>446</v>
@@ -33679,7 +33688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="453" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A453" s="2">
         <f t="shared" si="14"/>
         <v>447</v>
@@ -33749,7 +33758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="454" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A454" s="2">
         <f t="shared" si="14"/>
         <v>448</v>
@@ -33819,7 +33828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="455" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A455" s="2">
         <f t="shared" si="14"/>
         <v>449</v>
@@ -33889,7 +33898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="456" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A456" s="2">
         <f t="shared" si="14"/>
         <v>450</v>

</xml_diff>